<commit_message>
Vanhat backlogit lisätty, README päivitetty
</commit_message>
<xml_diff>
--- a/documents/Suunta_Sprint3_Backlog.xlsx
+++ b/documents/Suunta_Sprint3_Backlog.xlsx
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +622,7 @@
         <v>26</v>
       </c>
       <c r="G1" s="19">
-        <v>43066</v>
+        <v>43073</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>27</v>

</xml_diff>